<commit_message>
trigger agregados al diccionario de datos
</commit_message>
<xml_diff>
--- a/TP FINAL/Diccionario de datos.xlsx
+++ b/TP FINAL/Diccionario de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UADER\Tercero\Base de datos\TP FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61631661-1640-43F2-9869-C24FCF177379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2307CC17-63A2-4A6D-9C02-5350B656A6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{CC757FC8-D74E-49DC-81C4-0DBC941BD777}"/>
+    <workbookView minimized="1" xWindow="6912" yWindow="2772" windowWidth="5916" windowHeight="8904" activeTab="1" xr2:uid="{CC757FC8-D74E-49DC-81C4-0DBC941BD777}"/>
   </bookViews>
   <sheets>
     <sheet name="Dominios" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="181">
   <si>
     <t>Dominio</t>
   </si>
@@ -560,6 +560,24 @@
   </si>
   <si>
     <t>Regex para validar un mail</t>
+  </si>
+  <si>
+    <t>crearCarrito</t>
+  </si>
+  <si>
+    <t>Crea el carrito del usuario antes de crear el usuario</t>
+  </si>
+  <si>
+    <t>actualizarStockLibro</t>
+  </si>
+  <si>
+    <t>Luego de agregar una compra, se actualiza el stcok del libro del que se hizo la compra</t>
+  </si>
+  <si>
+    <t>actualizarLibroComprado</t>
+  </si>
+  <si>
+    <t>Luego de insertar un libro nuevo, se registra la compra en compra_libro</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFFCDC6-5958-4423-9092-CBC9157E6173}">
   <dimension ref="A2:H153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,6 +1105,7 @@
     <col min="3" max="3" width="17.5546875" customWidth="1"/>
     <col min="6" max="6" width="43.109375" customWidth="1"/>
     <col min="7" max="7" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="76.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1630,6 +1649,12 @@
       <c r="F33" t="s">
         <v>72</v>
       </c>
+      <c r="G33" t="s">
+        <v>179</v>
+      </c>
+      <c r="H33" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
@@ -1832,6 +1857,12 @@
       <c r="F45" t="s">
         <v>85</v>
       </c>
+      <c r="G45" t="s">
+        <v>177</v>
+      </c>
+      <c r="H45" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
@@ -2063,6 +2094,12 @@
       </c>
       <c r="F59" t="s">
         <v>112</v>
+      </c>
+      <c r="G59" t="s">
+        <v>175</v>
+      </c>
+      <c r="H59" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
TP FINAL base de datos terminado
</commit_message>
<xml_diff>
--- a/TP FINAL/Diccionario de datos.xlsx
+++ b/TP FINAL/Diccionario de datos.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UADER\Tercero\Base de datos\TP FINAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo\Desktop\escritorio\tercero\Base-de-datos\TP FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2307CC17-63A2-4A6D-9C02-5350B656A6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12439D4-227C-461A-87CF-692EE88D2705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6912" yWindow="2772" windowWidth="5916" windowHeight="8904" activeTab="1" xr2:uid="{CC757FC8-D74E-49DC-81C4-0DBC941BD777}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CC757FC8-D74E-49DC-81C4-0DBC941BD777}"/>
   </bookViews>
   <sheets>
     <sheet name="Dominios" sheetId="1" r:id="rId1"/>
-    <sheet name="Tablas" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
+    <sheet name="Tablas" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="192">
   <si>
     <t>Dominio</t>
   </si>
@@ -550,9 +551,6 @@
     <t>0 &lt;= x &lt;= 9.223.372.036.854.775.807</t>
   </si>
   <si>
-    <t>Tpunctuation</t>
-  </si>
-  <si>
     <t>parte entera: 0.00 &lt;= x &lt;= 4.294.967.295.99</t>
   </si>
   <si>
@@ -578,6 +576,42 @@
   </si>
   <si>
     <t>Luego de insertar un libro nuevo, se registra la compra en compra_libro</t>
+  </si>
+  <si>
+    <t>convertirLineaCarritoAOrden_detalle</t>
+  </si>
+  <si>
+    <t>Elimina la linea del carrito y lo transforma a una orden y orden detallada</t>
+  </si>
+  <si>
+    <t>opinion</t>
+  </si>
+  <si>
+    <t>comentario</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>Comentario del usuario</t>
+  </si>
+  <si>
+    <t>isbn del libro comentado</t>
+  </si>
+  <si>
+    <t>cuil del usuario que opino sobre el libro</t>
+  </si>
+  <si>
+    <t>FK (REFERENCES "cuil" - cuil), not null</t>
+  </si>
+  <si>
+    <t>Descripcion2</t>
+  </si>
+  <si>
+    <t>puntuacion</t>
+  </si>
+  <si>
+    <t>Tpuntuation</t>
   </si>
 </sst>
 </file>
@@ -672,7 +706,68 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="20">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -683,6 +778,346 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2F4A293-6657-4953-9155-C3004DE7E9C2}" name="Tabla1" displayName="Tabla1" ref="A2:H4" totalsRowShown="0">
+  <autoFilter ref="A2:H4" xr:uid="{A2F4A293-6657-4953-9155-C3004DE7E9C2}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{691303C9-D948-494C-8CC6-4FCB927C01CE}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{E7CFC41C-7DEB-4897-B68C-7A22CA036C14}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{E4C419A7-6AE6-4935-B49A-0B2869E10FED}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{48930109-5EEB-46CC-98F2-EDD358938A13}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{EB7E7D8C-3D5A-4CE9-9C9D-0FDDB3B79CB1}" name="Tamaño" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{55027C47-CDE5-41AE-A761-F2E0F57714DA}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{4ED7311E-1662-4FD0-A01B-019F7888D292}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{40C360ED-9567-42D4-A30F-843C432C2DE0}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9F17C108-610B-4F6E-9FD1-9520DC29FB9A}" name="Tabla10" displayName="Tabla10" ref="A50:H52" totalsRowShown="0">
+  <autoFilter ref="A50:H52" xr:uid="{9F17C108-610B-4F6E-9FD1-9520DC29FB9A}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{6615F8F1-6291-4202-9B39-DBC669650C2C}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{5D4B11D1-6B92-4679-9802-50A2CE76C270}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{1E914334-393A-4930-A30C-AE0314F59EDF}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{43FF032D-AD09-48E4-BE80-977E9487944A}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{9DAAD804-F9CC-4298-A94F-D1215688B59F}" name="Tamaño" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{AAE5A4C9-5541-416B-AA04-152A68B51D00}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{58DF25A1-C280-4842-904D-092659A5E3C6}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{E428869A-66B0-474C-8820-65E1903CF0F2}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F305AE5E-3385-42CF-8C9C-53A6E297951F}" name="Tabla11" displayName="Tabla11" ref="A54:H56" totalsRowShown="0">
+  <autoFilter ref="A54:H56" xr:uid="{F305AE5E-3385-42CF-8C9C-53A6E297951F}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{25A99ADF-A33B-4112-BD89-6C057CC1EA52}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{D8124C7F-98AE-457B-AE7B-1EB6CB877046}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{FDB7F174-1493-4AD4-A7C0-E349A3254AEC}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{483271E9-7013-4DC0-B22A-6D5923E9E079}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{58EC0675-B0D3-497E-A38F-C29E66A1D313}" name="Tamaño" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{07CD6AC4-4A12-4F57-A479-B609CB224771}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{429251A5-E716-4E19-B56C-FE3D4ECA1BAA}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{71621D3A-E33E-45FD-973D-35DE1F3E8937}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B1F06695-A75C-4810-898D-D89726E6CCAE}" name="Tabla12" displayName="Tabla12" ref="A58:H65" totalsRowShown="0">
+  <autoFilter ref="A58:H65" xr:uid="{B1F06695-A75C-4810-898D-D89726E6CCAE}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{A314A24A-1A81-40C3-B423-08279FEDE419}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{23F9F3DA-5EAA-4659-8397-D93C06C66C08}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{51ADBD92-FE68-4564-B50A-F0A10A9ED1F0}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{88F23D8F-01A9-4B1A-8053-7412327AFA91}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{1AE58F1D-F149-40BA-8E75-004FA633E37A}" name="Tamaño" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{E2C68613-6816-45FB-8984-31CA9A5D747E}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{9B4ACCF0-3600-4D7F-B5CB-BD8382F809C2}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{8B76152A-C65A-4D28-94BF-4E8A8D10EE07}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{585554F9-B19D-4480-8361-71C529508BF0}" name="Tabla13" displayName="Tabla13" ref="A67:H69" totalsRowShown="0">
+  <autoFilter ref="A67:H69" xr:uid="{585554F9-B19D-4480-8361-71C529508BF0}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{40F6C270-FA3B-4B2C-BADA-807D28BA0F70}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{5BB5B03D-2F42-4BE5-9540-4485CC90ADC7}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{AFDC2BF1-34B4-4286-91B3-DE9F13F33DE4}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{D0B34914-8580-46F7-9D43-70399D5BD982}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{BAB147DA-C908-4BF5-AD20-60FD4048F441}" name="Tamaño" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{B264E89F-A8E4-4FA4-9A3F-840721EBDBDC}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{EB58FB0D-C24E-425E-AF79-B4C7377FA821}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{A67F9B42-B807-4D34-9E36-76F4DAE65D74}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{834FADFE-7D2B-45A1-AE69-A7C8DD3892AF}" name="Tabla14" displayName="Tabla14" ref="A71:H75" totalsRowShown="0">
+  <autoFilter ref="A71:H75" xr:uid="{834FADFE-7D2B-45A1-AE69-A7C8DD3892AF}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{3760EBCD-5F3C-43B9-8667-B9BAEAD2B3B4}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{11231A14-55D1-4D2D-AF55-C9ECB7CCF848}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{891327D9-06D6-4831-AA37-C8611EC328CA}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{B47551AD-CE47-4100-A1BC-23D80E78D673}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{AFBF5D3A-101A-40B8-9A35-F646B922D24E}" name="Tamaño" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{B89AC1BA-EF27-4257-BC5E-AF821AEA5FB4}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{EB008E97-FA13-402E-A9D2-763EEFC1FC2C}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{5F623FE3-A878-457D-AC00-02D76628C85E}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{52DA74DE-D0C1-454F-9D79-21201532EA3A}" name="Tabla15" displayName="Tabla15" ref="A77:H83" totalsRowShown="0">
+  <autoFilter ref="A77:H83" xr:uid="{52DA74DE-D0C1-454F-9D79-21201532EA3A}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{229B9A2D-4498-413D-8353-73FE05A901F0}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{825F834D-9F16-491D-840E-356929425032}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{8E920895-093E-43AC-A298-F60E26D1665C}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{34F0134E-72CB-4FCE-BE11-13AED5B2C974}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{C8D1F161-A569-4DDB-8520-4CB01C0FA69D}" name="Tamaño" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{704FB56F-42CE-424C-9C84-F569A6B9A7DA}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{D561475D-55E5-4E04-A39A-7A4DF67AE183}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{5B9B05A2-56DE-4710-BE19-71955532A145}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{DAD17292-FDC7-4CF5-B1F7-E5AB4C6BED6E}" name="Tabla16" displayName="Tabla16" ref="A85:H88" totalsRowShown="0">
+  <autoFilter ref="A85:H88" xr:uid="{DAD17292-FDC7-4CF5-B1F7-E5AB4C6BED6E}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{6F994369-DF47-46CE-A108-9C31FC85B7D3}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{76C17928-8FDF-47D1-8659-C3E626D21A53}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{B8BF75AB-2DAB-4E27-9090-AD13FEEBD294}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{BA4DF770-4518-4E33-A00E-A8869F504855}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{C36BB985-87EC-4BB6-AB5E-2D50611A6C9B}" name="Tamaño" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{B938A64D-5929-4988-ACA8-789F8FA69A2C}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{49ECF8EF-723A-4390-A165-179558D50D40}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{E54BE5C2-C6B8-400C-9DEE-7BE480EEC19E}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{26328F98-0724-48AB-8143-3253673B66E5}" name="Tabla17" displayName="Tabla17" ref="A90:H96" totalsRowShown="0">
+  <autoFilter ref="A90:H96" xr:uid="{26328F98-0724-48AB-8143-3253673B66E5}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{7B2C759A-A05A-470A-9FAD-3150CAE9EA21}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{4674778A-73E4-4D31-95CB-CAED8FEC6D46}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{86A48820-5F86-4A28-8F5B-8187FB752B38}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{B214460F-D12A-4E9F-AEF3-9EB9C4E4B320}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{C12F6215-1DCB-490F-8B21-D4FA11EDEC24}" name="Tamaño" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{C7BA39AA-0B6A-426E-98C7-E520CC1E9B44}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{EDCCF1D2-3207-4DD3-855F-FA481DB540B8}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{0D42C037-2BD3-46C4-B18A-8B750905D21D}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{B53A1F68-7768-41BB-BFAE-253254F37D12}" name="Tabla18" displayName="Tabla18" ref="A98:H103" totalsRowShown="0">
+  <autoFilter ref="A98:H103" xr:uid="{B53A1F68-7768-41BB-BFAE-253254F37D12}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{24A27E13-777D-46D2-B9CF-CCB0D2CF7E11}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{E0ACC348-F33F-4B46-9755-E0ACD0B33B7A}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{076BA9F6-1100-4965-9C91-CCC51B179E21}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{63C39BFB-7213-410E-9677-BA14B9B4D79F}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{59650EDE-02F8-4C61-B781-0DBE30764909}" name="Tamaño" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{A20EEA12-E77F-487D-8AC8-A4290FF95CFD}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{27DE7F3B-1D5B-49A6-B509-96DA825E87F3}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{BF8CAB4A-975D-4080-876B-A3478D5F1660}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{C87D3401-0ABF-4288-ACAD-373A88EA7943}" name="Tabla19" displayName="Tabla19" ref="A105:H108" totalsRowShown="0">
+  <autoFilter ref="A105:H108" xr:uid="{C87D3401-0ABF-4288-ACAD-373A88EA7943}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{E071B2A2-A98E-4825-B4A0-02223B108EFE}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{19F5A4E1-B2FD-4360-9416-1FCB7DF9FF9D}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{95001A6B-30FA-47CF-8CEE-E2C39F0FDA55}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{CE949AA4-BF59-486A-B59E-E8F41B672F13}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{B72B77BD-6D2C-4D36-82C9-75D1C08B33BB}" name="Tamaño" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{1CCD37E0-F61B-4922-BA13-EDFD7F4EB67E}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{D67E9B7E-3F7D-4ACC-83D1-6380B0CEE2D9}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{7C1C219F-0780-4AB8-85FD-1A507B6261BE}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2588F6AF-4A3E-4FA7-A0D5-EF42F79A3AA9}" name="Tabla2" displayName="Tabla2" ref="A6:H9" totalsRowShown="0">
+  <autoFilter ref="A6:H9" xr:uid="{2588F6AF-4A3E-4FA7-A0D5-EF42F79A3AA9}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{76838891-0358-4438-89CB-3DC3160F0C30}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{A1C394CB-8439-4955-A113-271BCF920CF0}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{9EA47E2C-E133-4C18-912F-0DFEE50598E8}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{B93DEFDA-35C9-4AAD-9484-4F89F32C67C5}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{24BD2728-3793-471B-A2DC-77B5026B8CDD}" name="Tamaño" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{814502E7-DD60-42CE-8581-62658AB059F1}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{9EFA8419-6E5D-4FA6-9231-FB2BB63F3BAA}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{0601EDFD-159E-4337-9E9F-6294B33B85C2}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{1B0F1A59-2B2B-4DD2-8EF0-4F30A95A8EA4}" name="Tabla1921" displayName="Tabla1921" ref="A110:H113" totalsRowShown="0">
+  <autoFilter ref="A110:H113" xr:uid="{1B0F1A59-2B2B-4DD2-8EF0-4F30A95A8EA4}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{A6846E89-B891-4E45-BBD1-24320AF07036}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{A457B8A1-F120-4ECB-99CA-FF52AA7CABBB}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{3C7C3999-9092-48E7-8DFF-40438A67190E}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{5335015F-601A-406D-B0AC-BE150B9B49CC}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{284D8E00-AE22-4DD1-ACFC-0C0A2325B18D}" name="Tamaño" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{ECB1E748-91DF-4D73-8949-0EBB6B1CE91A}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{47CC009B-F631-42A9-8088-5E61574C5DDB}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{C9F5EDBA-4317-41E3-A233-C1BFBF5BEC8E}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CA14442-6CBE-4087-A269-B01DBE3C6756}" name="Tabla3" displayName="Tabla3" ref="A11:H14" totalsRowShown="0">
+  <autoFilter ref="A11:H14" xr:uid="{0CA14442-6CBE-4087-A269-B01DBE3C6756}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{0B2721E6-6424-4D5C-A69E-934F9797AFA8}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{77507AFF-3B33-4557-AF5A-10AD94C1D18B}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{4A330F06-B824-410C-AD59-456ADF2DF7DC}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{3AE9A3BC-ADD2-41D8-B51A-3869CB4CE75C}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{974DEC6B-02C9-46B6-9AB4-323422C62EA1}" name="Tamaño" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{2D6450AB-9295-47BF-AD6C-61BFF705B92B}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{60A1813F-F8BB-457F-8E5B-F0C8008BFDC4}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{C611D5D4-E443-46B8-B106-E3B6BF6AF5C3}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EF5A0213-EE78-48B0-B622-28E10E04C503}" name="Tabla4" displayName="Tabla4" ref="A16:H18" totalsRowShown="0">
+  <autoFilter ref="A16:H18" xr:uid="{EF5A0213-EE78-48B0-B622-28E10E04C503}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{9DBF5BE4-80C1-405D-8EDC-A661725C6BBA}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{9E723035-1474-4C61-9B2D-26FEE11497D9}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{941A5EF2-6049-4671-AFD0-10460D56DF79}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{AEA14754-EBFE-4D24-AED8-4156F1037F80}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{12F7AC39-596F-47EF-A7A8-DD1B778CA0B1}" name="Tamaño" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{AA6108E3-1A6B-427A-806E-9EBE40055E5D}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{3508B800-8A7C-41AB-9278-570771AB1720}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{2A344382-295D-4C0E-A60E-922400DCA7C6}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CF65CFFD-DEA9-4631-8D16-C190CF5DE8EE}" name="Tabla5" displayName="Tabla5" ref="A20:H22" totalsRowShown="0">
+  <autoFilter ref="A20:H22" xr:uid="{CF65CFFD-DEA9-4631-8D16-C190CF5DE8EE}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{75133378-42FF-4D2B-B8D2-D8B86B47847A}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{CF43FB1D-B131-41E4-AD86-134C8B8AF4AD}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{5A73602D-3042-4E63-A05D-BDBE8C56298A}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{B0014A2B-D4F1-4CAB-9C4E-60D581F107FD}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{03A7316F-2313-40DD-BF85-77FF4F295080}" name="Tamaño" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{7E27116C-42D1-468E-8934-6E184E1EBEC5}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{9B5F7133-D76D-4AB4-A7BD-32F191B35795}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{F7F4071C-AE6A-4694-9AC8-942E8454443B}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C34799A2-7687-46C8-BAF8-28F44A01618A}" name="Tabla6" displayName="Tabla6" ref="A24:H26" totalsRowShown="0">
+  <autoFilter ref="A24:H26" xr:uid="{C34799A2-7687-46C8-BAF8-28F44A01618A}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{FBDBE0E3-9561-4E1E-9EF0-4D010C490572}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{AC176D02-C31A-43A9-97FB-DF67B53A3FD9}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{B3E0496E-41C4-4738-B249-904A489F1B04}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{91EF1084-DF07-4B12-B255-FAA9C38E6DC8}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{B7E5E5C0-7D73-4CF5-A23D-88EFAF0B283A}" name="Tamaño" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{F335FCD8-655B-4E24-B725-F979DA70C634}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{DC3F470B-13D3-4350-A023-708C31BDCA0F}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{D01BD57A-B42B-4A8B-AFDB-2C1B1E44DD40}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6A744F25-738E-4ECE-B979-19B8212021B3}" name="Tabla7" displayName="Tabla7" ref="A28:H30" totalsRowShown="0">
+  <autoFilter ref="A28:H30" xr:uid="{6A744F25-738E-4ECE-B979-19B8212021B3}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{37E161ED-72AF-4025-85F9-350235BD0312}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{7749179A-7989-45DF-8C34-E0EB8944CCC5}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{D0AD1C00-7F17-46B0-816B-325374716BE2}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{A61359C4-05E2-4A94-9BAB-8A9582E97679}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{3C41CBB9-B399-49D8-B713-2079A49A0AF8}" name="Tamaño" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{31C5AB19-CE46-4EBA-A810-DF3A86ADE108}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{1911A8F6-91AB-4175-A964-005CE636B96C}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{5D675AB4-0D35-478F-92F6-A180BB7F3A74}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F95EFE9D-D415-450A-8CF3-49FFD916E186}" name="Tabla8" displayName="Tabla8" ref="A32:H42" totalsRowShown="0">
+  <autoFilter ref="A32:H42" xr:uid="{F95EFE9D-D415-450A-8CF3-49FFD916E186}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{9F788DF9-9CAD-4EC5-9910-4007E6E60B94}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{A4A72B1D-E510-4998-A28B-BB451098BA7D}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{52EA4C73-0863-4421-8501-5D81462033C8}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{BBC302F1-1F8E-4300-8678-7537C00575D9}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{421F26BB-F046-4297-922D-4DDEC363DCF9}" name="Tamaño" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{006F3A2F-984F-415B-B0F9-648D9E973E95}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{DFE96A36-38DA-43B8-B905-4EA94708D408}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{434BA1AE-D3CA-4BEC-85ED-2930149503B4}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F014ACBE-026C-484F-AD1A-F45B4D8A5706}" name="Tabla9" displayName="Tabla9" ref="A44:H48" totalsRowShown="0">
+  <autoFilter ref="A44:H48" xr:uid="{F014ACBE-026C-484F-AD1A-F45B4D8A5706}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D88BE3D2-D6FC-4616-BD5E-D9B515DA3E89}" name="Tabla"/>
+    <tableColumn id="2" xr3:uid="{CCBDBCBB-444E-40BF-8612-0639D0516E6B}" name="Restricciones"/>
+    <tableColumn id="3" xr3:uid="{E1C556D0-107D-43DC-8FAD-12F8A343BF19}" name="Atributos"/>
+    <tableColumn id="4" xr3:uid="{AD2E243C-30F2-4601-AC3D-62EFD1C4EB1C}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{3054AFB3-67A0-4BAA-90D6-3F330E4F03FD}" name="Tamaño" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{47675283-BD96-4DC4-BE6E-18291C378E6D}" name="Descripcion"/>
+    <tableColumn id="7" xr3:uid="{48F7B97A-8AD4-486A-8D20-9F76805D4BFC}" name="Triggers de la tabla"/>
+    <tableColumn id="8" xr3:uid="{4144DB45-47FD-4BFB-83CD-F947B5FD9DA7}" name="Descripcion2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -984,19 +1419,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4EAA0E-D449-4B85-BBA4-B8D2A94C0368}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="63.44140625" customWidth="1"/>
-    <col min="3" max="3" width="72.88671875" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" customWidth="1"/>
+    <col min="3" max="3" width="72.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>166</v>
       </c>
@@ -1018,7 +1453,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1029,7 +1464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1040,7 +1475,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1051,20 +1486,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -1073,15 +1508,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>169</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1091,24 +1526,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69CC800-0D1C-496B-8829-7EE81C8FFB49}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFFCDC6-5958-4423-9092-CBC9157E6173}">
   <dimension ref="A2:H153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView topLeftCell="A98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="39.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="6" max="6" width="43.109375" customWidth="1"/>
-    <col min="7" max="7" width="22.109375" customWidth="1"/>
-    <col min="8" max="8" width="76.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="43.140625" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1131,10 +1582,10 @@
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1154,7 +1605,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -1171,10 +1622,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1197,10 +1648,10 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1220,7 +1671,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -1237,7 +1688,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>90</v>
       </c>
@@ -1254,10 +1705,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1280,10 +1731,10 @@
         <v>20</v>
       </c>
       <c r="H11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1303,7 +1754,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -1320,7 +1771,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>89</v>
       </c>
@@ -1337,10 +1788,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1363,10 +1814,10 @@
         <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1386,7 +1837,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -1403,10 +1854,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1429,10 +1880,10 @@
         <v>20</v>
       </c>
       <c r="H20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1452,7 +1903,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>50</v>
       </c>
@@ -1469,10 +1920,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1495,10 +1946,10 @@
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1518,7 +1969,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>34</v>
       </c>
@@ -1535,10 +1986,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1561,10 +2012,10 @@
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1584,7 +2035,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>34</v>
       </c>
@@ -1601,10 +2052,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1627,10 +2078,10 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -1650,13 +2101,13 @@
         <v>72</v>
       </c>
       <c r="G33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H33" t="s">
         <v>179</v>
       </c>
-      <c r="H33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>50</v>
       </c>
@@ -1673,7 +2124,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>50</v>
       </c>
@@ -1690,7 +2141,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>50</v>
       </c>
@@ -1707,7 +2158,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>50</v>
       </c>
@@ -1724,7 +2175,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>50</v>
       </c>
@@ -1741,7 +2192,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>50</v>
       </c>
@@ -1758,7 +2209,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>70</v>
       </c>
@@ -1775,7 +2226,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>92</v>
       </c>
@@ -1792,7 +2243,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>93</v>
       </c>
@@ -1809,10 +2260,10 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -1835,10 +2286,10 @@
         <v>20</v>
       </c>
       <c r="H44" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -1858,13 +2309,13 @@
         <v>85</v>
       </c>
       <c r="G45" t="s">
+        <v>176</v>
+      </c>
+      <c r="H45" t="s">
         <v>177</v>
       </c>
-      <c r="H45" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>70</v>
       </c>
@@ -1881,7 +2332,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>91</v>
       </c>
@@ -1898,7 +2349,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>50</v>
       </c>
@@ -1915,10 +2366,10 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -1941,10 +2392,10 @@
         <v>20</v>
       </c>
       <c r="H50" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -1964,7 +2415,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>95</v>
       </c>
@@ -1981,10 +2432,10 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2007,10 +2458,10 @@
         <v>20</v>
       </c>
       <c r="H54" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>99</v>
       </c>
@@ -2030,7 +2481,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>70</v>
       </c>
@@ -2047,10 +2498,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -2073,10 +2524,10 @@
         <v>20</v>
       </c>
       <c r="H58" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>102</v>
       </c>
@@ -2096,13 +2547,13 @@
         <v>112</v>
       </c>
       <c r="G59" t="s">
+        <v>174</v>
+      </c>
+      <c r="H59" t="s">
         <v>175</v>
       </c>
-      <c r="H59" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>50</v>
       </c>
@@ -2119,7 +2570,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>50</v>
       </c>
@@ -2136,7 +2587,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>34</v>
       </c>
@@ -2153,7 +2604,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>49</v>
       </c>
@@ -2167,7 +2618,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>109</v>
       </c>
@@ -2184,7 +2635,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>108</v>
       </c>
@@ -2201,7 +2652,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -2224,10 +2675,10 @@
         <v>20</v>
       </c>
       <c r="H67" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>118</v>
       </c>
@@ -2247,7 +2698,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>123</v>
       </c>
@@ -2264,10 +2715,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E70" s="4"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -2290,10 +2741,10 @@
         <v>20</v>
       </c>
       <c r="H71" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>121</v>
       </c>
@@ -2312,8 +2763,14 @@
       <c r="F72" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G72" t="s">
+        <v>180</v>
+      </c>
+      <c r="H72" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>50</v>
       </c>
@@ -2330,7 +2787,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>123</v>
       </c>
@@ -2347,7 +2804,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>108</v>
       </c>
@@ -2364,10 +2821,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E76" s="4"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -2390,10 +2847,10 @@
         <v>20</v>
       </c>
       <c r="H77" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>128</v>
       </c>
@@ -2413,7 +2870,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>50</v>
       </c>
@@ -2430,7 +2887,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>50</v>
       </c>
@@ -2447,7 +2904,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>24</v>
       </c>
@@ -2464,7 +2921,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>119</v>
       </c>
@@ -2481,7 +2938,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>134</v>
       </c>
@@ -2498,11 +2955,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B84" s="5"/>
       <c r="E84" s="4"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -2525,10 +2982,10 @@
         <v>20</v>
       </c>
       <c r="H85" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>140</v>
       </c>
@@ -2548,7 +3005,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>50</v>
       </c>
@@ -2565,7 +3022,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>109</v>
       </c>
@@ -2582,10 +3039,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>15</v>
       </c>
@@ -2608,10 +3065,10 @@
         <v>20</v>
       </c>
       <c r="H90" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>145</v>
       </c>
@@ -2631,7 +3088,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>50</v>
       </c>
@@ -2648,7 +3105,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>50</v>
       </c>
@@ -2665,7 +3122,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>155</v>
       </c>
@@ -2682,7 +3139,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>119</v>
       </c>
@@ -2699,7 +3156,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>151</v>
       </c>
@@ -2716,10 +3173,10 @@
         <v>157</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E97" s="4"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>15</v>
       </c>
@@ -2742,10 +3199,10 @@
         <v>20</v>
       </c>
       <c r="H98" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>158</v>
       </c>
@@ -2765,7 +3222,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>50</v>
       </c>
@@ -2782,7 +3239,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>50</v>
       </c>
@@ -2799,7 +3256,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>160</v>
       </c>
@@ -2816,7 +3273,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>123</v>
       </c>
@@ -2833,158 +3290,310 @@
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E105" s="4"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E106" s="4"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E107" s="4"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E108" s="4"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>15</v>
+      </c>
+      <c r="B105" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105" t="s">
+        <v>17</v>
+      </c>
+      <c r="D105" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" t="s">
+        <v>19</v>
+      </c>
+      <c r="F105" t="s">
+        <v>2</v>
+      </c>
+      <c r="G105" t="s">
+        <v>20</v>
+      </c>
+      <c r="H105" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>182</v>
+      </c>
+      <c r="C106" t="s">
+        <v>183</v>
+      </c>
+      <c r="D106" t="s">
+        <v>184</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F106" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>123</v>
+      </c>
+      <c r="C107" t="s">
+        <v>60</v>
+      </c>
+      <c r="D107" t="s">
+        <v>184</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F107" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>188</v>
+      </c>
+      <c r="C108" t="s">
+        <v>103</v>
+      </c>
+      <c r="D108" t="s">
+        <v>5</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F108" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E110" s="4"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E111" s="4"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E112" s="4"/>
-    </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E113" s="4"/>
-    </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>15</v>
+      </c>
+      <c r="B110" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110" t="s">
+        <v>17</v>
+      </c>
+      <c r="D110" t="s">
+        <v>18</v>
+      </c>
+      <c r="E110" t="s">
+        <v>19</v>
+      </c>
+      <c r="F110" t="s">
+        <v>2</v>
+      </c>
+      <c r="G110" t="s">
+        <v>20</v>
+      </c>
+      <c r="H110" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>190</v>
+      </c>
+      <c r="C111" t="s">
+        <v>190</v>
+      </c>
+      <c r="D111" t="s">
+        <v>191</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F111" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>123</v>
+      </c>
+      <c r="C112" t="s">
+        <v>60</v>
+      </c>
+      <c r="D112" t="s">
+        <v>184</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F112" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>188</v>
+      </c>
+      <c r="C113" t="s">
+        <v>103</v>
+      </c>
+      <c r="D113" t="s">
+        <v>5</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F113" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E153" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="20">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId21"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TP FINAL ARREGLADO Y TERMINADO
</commit_message>
<xml_diff>
--- a/TP FINAL/Diccionario de datos.xlsx
+++ b/TP FINAL/Diccionario de datos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo\Desktop\escritorio\tercero\Base-de-datos\TP FINAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UADER\Tercero\Base de datos\TP FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12439D4-227C-461A-87CF-692EE88D2705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EC62EB-AA5C-40EB-A832-330FF0721B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CC757FC8-D74E-49DC-81C4-0DBC941BD777}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{CC757FC8-D74E-49DC-81C4-0DBC941BD777}"/>
   </bookViews>
   <sheets>
     <sheet name="Dominios" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
-    <sheet name="Tablas" sheetId="2" r:id="rId3"/>
+    <sheet name="Tablas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="202">
   <si>
     <t>Dominio</t>
   </si>
@@ -612,6 +611,36 @@
   </si>
   <si>
     <t>Tpuntuation</t>
+  </si>
+  <si>
+    <t>minAMayus</t>
+  </si>
+  <si>
+    <t>Pasa el nombre del idioma a mayusculas</t>
+  </si>
+  <si>
+    <t>Pasa el nombre de la ciudad a mayusculas</t>
+  </si>
+  <si>
+    <t>Pasa el nombre de la provincia a mayusculas</t>
+  </si>
+  <si>
+    <t>Pasa el nombre del pais a mayusculas</t>
+  </si>
+  <si>
+    <t>Pasa el nombre del autor a mayusculas</t>
+  </si>
+  <si>
+    <t>Pasa el nombre del tema a mayusculas</t>
+  </si>
+  <si>
+    <t>Pasa el nombre de la editorial a mayusculas</t>
+  </si>
+  <si>
+    <t>minAMayusCorreo</t>
+  </si>
+  <si>
+    <t>Pasa el correo a mayusculas</t>
   </si>
 </sst>
 </file>
@@ -1419,19 +1448,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4EAA0E-D449-4B85-BBA4-B8D2A94C0368}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="63.42578125" customWidth="1"/>
-    <col min="3" max="3" width="72.85546875" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="63.44140625" customWidth="1"/>
+    <col min="3" max="3" width="72.88671875" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>166</v>
       </c>
@@ -1453,7 +1482,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1464,7 +1493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1475,7 +1504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1486,7 +1515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1497,7 +1526,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>191</v>
       </c>
@@ -1508,7 +1537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>169</v>
       </c>
@@ -1526,40 +1555,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69CC800-0D1C-496B-8829-7EE81C8FFB49}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFFCDC6-5958-4423-9092-CBC9157E6173}">
   <dimension ref="A2:H153"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView tabSelected="1" topLeftCell="D49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="43.140625" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" customWidth="1"/>
-    <col min="8" max="8" width="76.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="39.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="43.109375" customWidth="1"/>
+    <col min="7" max="7" width="33.44140625" customWidth="1"/>
+    <col min="8" max="8" width="76.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1585,7 +1600,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1604,8 +1619,14 @@
       <c r="F3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -1622,10 +1643,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1651,7 +1672,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1670,8 +1691,14 @@
       <c r="F7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -1688,7 +1715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>90</v>
       </c>
@@ -1705,10 +1732,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1734,7 +1761,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1753,8 +1780,14 @@
       <c r="F12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -1771,7 +1804,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>89</v>
       </c>
@@ -1788,10 +1821,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1817,7 +1850,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1836,8 +1869,14 @@
       <c r="F17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>192</v>
+      </c>
+      <c r="H17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -1854,10 +1893,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1883,7 +1922,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1902,8 +1941,14 @@
       <c r="F21" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>192</v>
+      </c>
+      <c r="H21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>50</v>
       </c>
@@ -1920,10 +1965,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1949,7 +1994,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1968,8 +2013,14 @@
       <c r="F25" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>34</v>
       </c>
@@ -1986,10 +2037,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2015,7 +2066,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2034,8 +2085,14 @@
       <c r="F29" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>192</v>
+      </c>
+      <c r="H29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>34</v>
       </c>
@@ -2052,10 +2109,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -2081,7 +2138,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -2107,7 +2164,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>50</v>
       </c>
@@ -2124,7 +2181,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>50</v>
       </c>
@@ -2141,7 +2198,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>50</v>
       </c>
@@ -2158,7 +2215,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>50</v>
       </c>
@@ -2175,7 +2232,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>50</v>
       </c>
@@ -2192,7 +2249,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>50</v>
       </c>
@@ -2209,7 +2266,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>70</v>
       </c>
@@ -2226,7 +2283,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>92</v>
       </c>
@@ -2243,7 +2300,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>93</v>
       </c>
@@ -2260,10 +2317,10 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -2289,7 +2346,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -2315,7 +2372,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>70</v>
       </c>
@@ -2332,7 +2389,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>91</v>
       </c>
@@ -2349,7 +2406,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>50</v>
       </c>
@@ -2366,10 +2423,10 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -2395,7 +2452,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -2415,7 +2472,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>95</v>
       </c>
@@ -2432,10 +2489,10 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2461,7 +2518,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>99</v>
       </c>
@@ -2481,7 +2538,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>70</v>
       </c>
@@ -2498,10 +2555,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -2527,7 +2584,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>102</v>
       </c>
@@ -2553,7 +2610,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>50</v>
       </c>
@@ -2569,8 +2626,14 @@
       <c r="F60" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>200</v>
+      </c>
+      <c r="H60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>50</v>
       </c>
@@ -2587,7 +2650,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>34</v>
       </c>
@@ -2604,7 +2667,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
         <v>49</v>
       </c>
@@ -2618,7 +2681,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>109</v>
       </c>
@@ -2635,7 +2698,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>108</v>
       </c>
@@ -2652,7 +2715,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -2678,7 +2741,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>118</v>
       </c>
@@ -2698,7 +2761,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>123</v>
       </c>
@@ -2715,10 +2778,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E70" s="4"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -2744,7 +2807,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>121</v>
       </c>
@@ -2770,7 +2833,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>50</v>
       </c>
@@ -2787,7 +2850,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>123</v>
       </c>
@@ -2804,7 +2867,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>108</v>
       </c>
@@ -2821,10 +2884,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E76" s="4"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -2850,7 +2913,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>128</v>
       </c>
@@ -2870,7 +2933,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>50</v>
       </c>
@@ -2887,7 +2950,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>50</v>
       </c>
@@ -2904,7 +2967,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>24</v>
       </c>
@@ -2921,7 +2984,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>119</v>
       </c>
@@ -2938,7 +3001,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>134</v>
       </c>
@@ -2955,11 +3018,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B84" s="5"/>
       <c r="E84" s="4"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -2985,7 +3048,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>140</v>
       </c>
@@ -3005,7 +3068,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>50</v>
       </c>
@@ -3022,7 +3085,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>109</v>
       </c>
@@ -3039,10 +3102,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>15</v>
       </c>
@@ -3068,7 +3131,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>145</v>
       </c>
@@ -3088,7 +3151,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>50</v>
       </c>
@@ -3105,7 +3168,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>50</v>
       </c>
@@ -3122,7 +3185,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>155</v>
       </c>
@@ -3139,7 +3202,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>119</v>
       </c>
@@ -3156,7 +3219,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>151</v>
       </c>
@@ -3173,10 +3236,10 @@
         <v>157</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E97" s="4"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>15</v>
       </c>
@@ -3202,7 +3265,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>158</v>
       </c>
@@ -3222,7 +3285,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>50</v>
       </c>
@@ -3239,7 +3302,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>50</v>
       </c>
@@ -3256,7 +3319,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>160</v>
       </c>
@@ -3273,7 +3336,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>123</v>
       </c>
@@ -3290,10 +3353,10 @@
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>15</v>
       </c>
@@ -3319,7 +3382,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>182</v>
       </c>
@@ -3336,7 +3399,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>123</v>
       </c>
@@ -3353,7 +3416,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>188</v>
       </c>
@@ -3370,10 +3433,10 @@
         <v>187</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>15</v>
       </c>
@@ -3399,7 +3462,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>190</v>
       </c>
@@ -3416,7 +3479,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>123</v>
       </c>
@@ -3433,7 +3496,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>188</v>
       </c>
@@ -3450,124 +3513,124 @@
         <v>187</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E153" s="4"/>
     </row>
   </sheetData>

</xml_diff>